<commit_message>
Présentation Procédures stockées / Exercices Fil Rouge
</commit_message>
<xml_diff>
--- a/Planning/Feuilles de route/Feuilles_de_route_08_28.xlsx
+++ b/Planning/Feuilles de route/Feuilles_de_route_08_28.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fef\Documents\DWWM_22238\ressources\Planning\Feuilles de route\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{655A3A25-6CBF-442D-9855-B2455D3753D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94F8D8F-A8F8-4A6B-ABE8-C23BEE096B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Lundi</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Semaine du 29/08 au 01/09</t>
+  </si>
+  <si>
+    <t>Dépôts BDD FIL ROUGE: 16h</t>
   </si>
 </sst>
 </file>
@@ -347,28 +350,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -687,7 +690,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -727,25 +732,25 @@
       <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="19" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="20" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="12"/>
-      <c r="F4" s="20"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:7" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="18"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -758,7 +763,9 @@
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="F6" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>